<commit_message>
highlight of significant  coefficients
</commit_message>
<xml_diff>
--- a/regs/results_tables.xlsx
+++ b/regs/results_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michel\Google Drive\DOUTORADO FGV\Artigos\EC 29-2000\ec29\regs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C5A30A-55B3-41F9-A43B-2CFC99EBB44A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD0C02B-40E3-47BC-BAB4-F0C066F19187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4470" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="first_stage" sheetId="8" r:id="rId1"/>
@@ -3674,7 +3674,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>